<commit_message>
added last few changes
</commit_message>
<xml_diff>
--- a/checking_endogenous_sorting_manually.xlsx
+++ b/checking_endogenous_sorting_manually.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acf23f56b39cff3f/Otree - Sharing/PGG_sorting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguido\Documents\GitHub\Endogenous_Exogenous_Group_Formation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{F32ED2ED-3646-4673-A291-E393921A4F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFE2FB12-5216-42D7-92D0-3117B7887E74}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D5A6CE-1D10-4142-840A-FA75315C8293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{200E2B7D-B07B-438B-BE85-59EF936DB904}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{200E2B7D-B07B-438B-BE85-59EF936DB904}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -406,13 +406,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A001C47A-AD03-4D0F-B0B4-8D8F9F57836A}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1">
@@ -583,6 +583,39 @@
       <c r="K7">
         <f>SUM(D4:E5)+SUM(A4:A5)+SUM(D1:E1)</f>
         <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>